<commit_message>
adding more config files for GTY and GTH
</commit_message>
<xml_diff>
--- a/examples/apex_USp/src/xcku15p-ffva1760-2_GTY.xlsx
+++ b/examples/apex_USp/src/xcku15p-ffva1760-2_GTY.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="US+_GTY_tx_rx" sheetId="1" state="visible" r:id="rId2"/>
@@ -5586,7 +5586,7 @@
   <dimension ref="A1:F829"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A745" activeCellId="0" sqref="A745"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12203,8 +12203,8 @@
   </sheetPr>
   <dimension ref="A1:M311"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19992,8 +19992,8 @@
   </sheetPr>
   <dimension ref="A1:G812"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B622" activeCellId="0" sqref="B622"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A780" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D237" activeCellId="0" sqref="D237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>